<commit_message>
added some error handling to all files
</commit_message>
<xml_diff>
--- a/backend/exports/report-2025-12.xlsx
+++ b/backend/exports/report-2025-12.xlsx
@@ -19,13 +19,13 @@
     <t>Total</t>
   </si>
   <si>
+    <t>Transport</t>
+  </si>
+  <si>
     <t>Food</t>
   </si>
   <si>
     <t>Bills</t>
-  </si>
-  <si>
-    <t>Transport</t>
   </si>
   <si>
     <t>Budget</t>
@@ -435,7 +435,7 @@
         <v>2</v>
       </c>
       <c r="B2">
-        <v>143</v>
+        <v>156</v>
       </c>
     </row>
     <row r="3" spans="1:2" x14ac:dyDescent="0.25">
@@ -443,7 +443,7 @@
         <v>3</v>
       </c>
       <c r="B3">
-        <v>300</v>
+        <v>143</v>
       </c>
     </row>
     <row r="4" spans="1:2" x14ac:dyDescent="0.25">
@@ -451,7 +451,7 @@
         <v>4</v>
       </c>
       <c r="B4">
-        <v>156</v>
+        <v>900</v>
       </c>
     </row>
     <row r="6" spans="1:2" x14ac:dyDescent="0.25">
@@ -467,7 +467,7 @@
         <v>6</v>
       </c>
       <c r="B7">
-        <v>599</v>
+        <v>1199</v>
       </c>
     </row>
     <row r="8" spans="1:2" x14ac:dyDescent="0.25">
@@ -475,7 +475,7 @@
         <v>7</v>
       </c>
       <c r="B8">
-        <v>549401</v>
+        <v>548801</v>
       </c>
     </row>
   </sheetData>

</xml_diff>